<commit_message>
add global coms. Also fix local echo
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +483,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -494,10 +494,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -516,10 +516,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -527,10 +527,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -538,10 +538,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -549,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="C11" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -560,10 +560,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="C12" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -571,10 +571,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -582,10 +582,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -593,10 +593,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="C15" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -604,10 +604,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="C16" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -615,10 +615,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="C17" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -626,10 +626,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C18" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -637,10 +637,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C19" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -648,10 +648,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="C20" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -659,10 +659,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C21" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
@@ -670,10 +670,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C22" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -681,10 +681,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C23" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -692,10 +692,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C24" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -703,10 +703,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C25" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
@@ -714,10 +714,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C26" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -725,10 +725,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C27" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -736,10 +736,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C28" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -747,10 +747,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C29" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
@@ -758,10 +758,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C30" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -769,10 +769,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C31" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -780,10 +780,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C32" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -791,10 +791,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C33" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -802,10 +802,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C34" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -813,10 +813,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C35" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -824,10 +824,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C36" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -835,10 +835,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C37" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -846,10 +846,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C38" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -857,10 +857,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C39" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -868,10 +868,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C40" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -879,10 +879,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C41" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
@@ -890,10 +890,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C42" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
@@ -901,10 +901,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C43" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
@@ -912,10 +912,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C44" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
@@ -923,10 +923,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C45" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
@@ -934,10 +934,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C46" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
@@ -945,10 +945,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C47" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
@@ -956,10 +956,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C48" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -967,10 +967,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C49" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
@@ -978,10 +978,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C50" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -989,10 +989,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C51" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
@@ -1000,10 +1000,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C52" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -1011,10 +1011,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C53" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
@@ -1025,7 +1025,7 @@
         <v>3</v>
       </c>
       <c r="C54" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
@@ -1036,7 +1036,7 @@
         <v>3</v>
       </c>
       <c r="C55" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
@@ -1044,10 +1044,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C56" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57">
@@ -1055,10 +1055,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C57" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58">
@@ -1066,10 +1066,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C58" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
@@ -1077,10 +1077,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C59" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60">
@@ -1088,10 +1088,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C60" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
@@ -1099,10 +1099,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C61" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
@@ -1110,10 +1110,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C62" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
@@ -1121,10 +1121,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C63" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -1132,10 +1132,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C64" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65">
@@ -1143,10 +1143,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C65" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66">
@@ -1154,10 +1154,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C66" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
@@ -1165,10 +1165,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C67" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -1176,10 +1176,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C68" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -1187,10 +1187,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C69" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
@@ -1198,10 +1198,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C70" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -1209,10 +1209,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C71" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
@@ -1220,10 +1220,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C72" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -1231,10 +1231,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C73" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74">
@@ -1242,10 +1242,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C74" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75">
@@ -1253,10 +1253,1132 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
+        <v>3</v>
+      </c>
+      <c r="C75" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>3</v>
+      </c>
+      <c r="C76" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>3</v>
+      </c>
+      <c r="C77" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="n">
+        <v>3</v>
+      </c>
+      <c r="C78" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="n">
+        <v>3</v>
+      </c>
+      <c r="C79" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="n">
+        <v>3</v>
+      </c>
+      <c r="C80" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="n">
+        <v>3</v>
+      </c>
+      <c r="C81" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="n">
+        <v>3</v>
+      </c>
+      <c r="C82" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="n">
+        <v>3</v>
+      </c>
+      <c r="C83" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="n">
+        <v>3</v>
+      </c>
+      <c r="C84" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="n">
+        <v>3</v>
+      </c>
+      <c r="C85" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="n">
+        <v>3</v>
+      </c>
+      <c r="C86" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="n">
+        <v>3</v>
+      </c>
+      <c r="C87" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="n">
+        <v>3</v>
+      </c>
+      <c r="C88" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="n">
+        <v>3</v>
+      </c>
+      <c r="C89" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="n">
+        <v>3</v>
+      </c>
+      <c r="C90" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="n">
+        <v>3</v>
+      </c>
+      <c r="C91" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="n">
+        <v>3</v>
+      </c>
+      <c r="C92" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="n">
+        <v>3</v>
+      </c>
+      <c r="C93" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="n">
+        <v>3</v>
+      </c>
+      <c r="C94" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="n">
+        <v>3</v>
+      </c>
+      <c r="C95" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="n">
+        <v>3</v>
+      </c>
+      <c r="C96" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="n">
+        <v>3</v>
+      </c>
+      <c r="C97" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="n">
+        <v>3</v>
+      </c>
+      <c r="C98" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="n">
+        <v>3</v>
+      </c>
+      <c r="C99" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="n">
+        <v>3</v>
+      </c>
+      <c r="C100" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="n">
+        <v>3</v>
+      </c>
+      <c r="C101" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="n">
+        <v>3</v>
+      </c>
+      <c r="C102" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="n">
+        <v>3</v>
+      </c>
+      <c r="C103" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="n">
+        <v>3</v>
+      </c>
+      <c r="C104" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="n">
+        <v>3</v>
+      </c>
+      <c r="C105" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="n">
+        <v>3</v>
+      </c>
+      <c r="C106" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="n">
+        <v>3</v>
+      </c>
+      <c r="C107" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="n">
+        <v>3</v>
+      </c>
+      <c r="C108" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="n">
+        <v>3</v>
+      </c>
+      <c r="C109" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="n">
+        <v>3</v>
+      </c>
+      <c r="C110" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="n">
+        <v>3</v>
+      </c>
+      <c r="C111" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="n">
+        <v>3</v>
+      </c>
+      <c r="C112" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="n">
+        <v>3</v>
+      </c>
+      <c r="C113" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="n">
+        <v>3</v>
+      </c>
+      <c r="C114" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="n">
+        <v>3</v>
+      </c>
+      <c r="C115" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="n">
+        <v>3</v>
+      </c>
+      <c r="C116" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="n">
+        <v>3</v>
+      </c>
+      <c r="C117" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="n">
+        <v>3</v>
+      </c>
+      <c r="C118" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="n">
+        <v>3</v>
+      </c>
+      <c r="C119" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="n">
+        <v>3</v>
+      </c>
+      <c r="C120" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="n">
+        <v>3</v>
+      </c>
+      <c r="C121" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="n">
+        <v>3</v>
+      </c>
+      <c r="C122" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="n">
+        <v>3</v>
+      </c>
+      <c r="C123" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="n">
+        <v>3</v>
+      </c>
+      <c r="C124" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="n">
+        <v>3</v>
+      </c>
+      <c r="C125" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="n">
+        <v>3</v>
+      </c>
+      <c r="C126" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="n">
+        <v>3</v>
+      </c>
+      <c r="C127" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="n">
+        <v>3</v>
+      </c>
+      <c r="C128" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="n">
+        <v>3</v>
+      </c>
+      <c r="C129" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="n">
+        <v>3</v>
+      </c>
+      <c r="C130" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="n">
+        <v>3</v>
+      </c>
+      <c r="C131" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="n">
+        <v>3</v>
+      </c>
+      <c r="C132" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="n">
+        <v>3</v>
+      </c>
+      <c r="C133" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="n">
+        <v>3</v>
+      </c>
+      <c r="C134" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="n">
+        <v>3</v>
+      </c>
+      <c r="C135" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="n">
+        <v>3</v>
+      </c>
+      <c r="C136" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="n">
+        <v>3</v>
+      </c>
+      <c r="C137" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="n">
+        <v>3</v>
+      </c>
+      <c r="C138" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="n">
+        <v>3</v>
+      </c>
+      <c r="C139" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="n">
+        <v>3</v>
+      </c>
+      <c r="C140" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="n">
+        <v>3</v>
+      </c>
+      <c r="C141" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="n">
+        <v>3</v>
+      </c>
+      <c r="C142" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="n">
+        <v>3</v>
+      </c>
+      <c r="C143" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="n">
+        <v>3</v>
+      </c>
+      <c r="C144" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="n">
+        <v>3</v>
+      </c>
+      <c r="C145" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="n">
+        <v>4</v>
+      </c>
+      <c r="C146" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="n">
+        <v>4</v>
+      </c>
+      <c r="C147" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="n">
+        <v>4</v>
+      </c>
+      <c r="C148" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="n">
+        <v>4</v>
+      </c>
+      <c r="C149" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="n">
+        <v>4</v>
+      </c>
+      <c r="C150" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="n">
+        <v>4</v>
+      </c>
+      <c r="C151" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="n">
+        <v>4</v>
+      </c>
+      <c r="C152" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" t="n">
+        <v>4</v>
+      </c>
+      <c r="C153" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" t="n">
+        <v>4</v>
+      </c>
+      <c r="C154" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" t="n">
+        <v>4</v>
+      </c>
+      <c r="C155" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" t="n">
+        <v>4</v>
+      </c>
+      <c r="C156" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" t="n">
+        <v>4</v>
+      </c>
+      <c r="C157" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="n">
+        <v>4</v>
+      </c>
+      <c r="C158" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" t="n">
+        <v>4</v>
+      </c>
+      <c r="C159" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="n">
+        <v>4</v>
+      </c>
+      <c r="C160" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B161" t="n">
+        <v>4</v>
+      </c>
+      <c r="C161" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" t="n">
+        <v>4</v>
+      </c>
+      <c r="C162" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" t="n">
+        <v>4</v>
+      </c>
+      <c r="C163" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="n">
+        <v>4</v>
+      </c>
+      <c r="C164" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="n">
+        <v>4</v>
+      </c>
+      <c r="C165" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" t="n">
+        <v>4</v>
+      </c>
+      <c r="C166" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B167" t="n">
+        <v>4</v>
+      </c>
+      <c r="C167" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B168" t="n">
+        <v>6</v>
+      </c>
+      <c r="C168" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B169" t="n">
+        <v>6</v>
+      </c>
+      <c r="C169" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B170" t="n">
+        <v>6</v>
+      </c>
+      <c r="C170" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="B171" t="n">
+        <v>6</v>
+      </c>
+      <c r="C171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B172" t="n">
+        <v>6</v>
+      </c>
+      <c r="C172" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B173" t="n">
+        <v>6</v>
+      </c>
+      <c r="C173" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B174" t="n">
+        <v>6</v>
+      </c>
+      <c r="C174" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B175" t="n">
+        <v>6</v>
+      </c>
+      <c r="C175" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B176" t="n">
+        <v>6</v>
+      </c>
+      <c r="C176" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="n">
+        <v>6</v>
+      </c>
+      <c r="C177" t="n">
         <v>0</v>
-      </c>
-      <c r="C75" t="n">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>